<commit_message>
ZSS-260:  * fix resolving the formulas of validation constraint bug  * fix Date object doesn't convert to Excel date type issue when validating  * fix default day value to 0 when parsing a pure time pattern  * fix throwing exception when rendering in Excel 97-2003 file  * modify and add test cases
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue/260-validation.xlsx
+++ b/zss.test/src/main/webapp/issue/260-validation.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="17460" windowHeight="9465" tabRatio="781"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="17460" windowHeight="9465" tabRatio="781" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Validation" sheetId="10" r:id="rId1"/>
+    <sheet name="datetime" sheetId="11" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Alex</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,16 +47,100 @@
   <si>
     <t>&lt;-Input</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;-Input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List (constants with comma)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;-Input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Are they equal ?</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date / Time</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>In number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input below</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>In number</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>input following text into cells:
+  3:21
+  1/23/2013
+  1/23/13 3:21
+  1/1/2012</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;- time only</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;- date only</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;- date and time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;- custom: yyyy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="177" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="178" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="179" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="180" formatCode="h:mm;@"/>
+    <numFmt numFmtId="181" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="182" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="6">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,20 +152,42 @@
     <font>
       <sz val="9"/>
       <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -88,25 +195,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -398,16 +581,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:K5"/>
+  <dimension ref="B3:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="8" max="11" width="14" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11">
@@ -417,10 +599,10 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>10</v>
       </c>
     </row>
@@ -431,16 +613,16 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -448,27 +630,75 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="3"/>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>41275</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>41305</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="4">
+        <v>41275.041666666664</v>
+      </c>
+      <c r="I7" s="4">
+        <v>41275.333333333336</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
-      <formula1>$H$4:$K$4</formula1>
-    </dataValidation>
+  <dataValidations count="7">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>H3</formula1>
       <formula2>I3</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
       <formula1>41275</formula1>
       <formula2>41639</formula2>
     </dataValidation>
@@ -476,8 +706,169 @@
       <formula1>H5</formula1>
       <formula2>I5</formula2>
     </dataValidation>
+    <dataValidation type="list" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+      <formula1>"1,3,5,7"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+      <formula1>$H$4:$K$4</formula1>
+    </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
+      <formula1>H7</formula1>
+      <formula2>I7</formula2>
+    </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+      <formula1>H8</formula1>
+      <formula2>I8</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="4" width="18.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="92.25" customHeight="1">
+      <c r="C2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="6" t="b">
+        <f>C5=D5</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="8">
+        <v>0.13958333333333334</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="6" t="b">
+        <f>C6=D6</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="10">
+        <v>41297</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="6" t="b">
+        <f>C7=D7</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="11">
+        <v>41297.13958333333</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="6" t="b">
+        <f>C8=D8</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="17">
+        <v>40909</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="12"/>
+      <c r="C9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="12"/>
+      <c r="C10" s="9">
+        <f>C5</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <f>D5</f>
+        <v>0.13958333333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="12"/>
+      <c r="C11" s="9">
+        <f>C6</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <f>D6</f>
+        <v>41297</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="12"/>
+      <c r="C12" s="9">
+        <f>C7</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="9">
+        <f>D7</f>
+        <v>41297.13958333333</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="C13" s="9">
+        <f>C8</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <f>D8</f>
+        <v>40909</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>